<commit_message>
Keyword Driven Framework - 2 samples
</commit_message>
<xml_diff>
--- a/DataDrivenFrameWorkExample2/src/dataEngine/DataEngine.xlsx
+++ b/DataDrivenFrameWorkExample2/src/dataEngine/DataEngine.xlsx
@@ -8,16 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://boozallen-my.sharepoint.com/personal/625337_bah_com/Documents/Documents/Personal/Trainings/Selenium/Workspaces/Feb2023/DataDrivenFrameWorkExample2/src/dataEngine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{85F8412F-80C7-43F8-83CE-0D26DDE02805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6F8F147-70D9-43CF-A959-3209B3E15007}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{3F956BA8-EE34-4E14-AB61-110242D9F3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E2A1174-51DA-411C-815F-E43E15890EA7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40914548-F9A3-4D3F-B989-9A3EE95A24BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{40914548-F9A3-4D3F-B989-9A3EE95A24BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="7" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="8" r:id="rId2"/>
-    <sheet name="Template" sheetId="5" r:id="rId3"/>
-    <sheet name="Test Steps-OLD" sheetId="6" r:id="rId4"/>
+    <sheet name="Settings" sheetId="9" r:id="rId3"/>
+    <sheet name="Keywords" sheetId="10" r:id="rId4"/>
+    <sheet name="Template" sheetId="5" r:id="rId5"/>
+    <sheet name="Test Steps-OLD" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="Action_Keywords">Settings!$D$2:$D$7</definedName>
+    <definedName name="Home_Page">Settings!$C$2:$C$7</definedName>
+    <definedName name="Login_Page">Settings!$B$2:$B$7</definedName>
+    <definedName name="Page_name">Settings!$A$2:$A$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="88">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -147,9 +155,6 @@
     <t>click_Logout</t>
   </si>
   <si>
-    <t>input_Username</t>
-  </si>
-  <si>
     <t>txtbx_UserName</t>
   </si>
   <si>
@@ -181,13 +186,136 @@
   </si>
   <si>
     <t>LogIn_02</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Data Set</t>
+  </si>
+  <si>
+    <t>chuy@bah.com</t>
+  </si>
+  <si>
+    <t>Hello1234!</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>chuy2@bah.com</t>
+  </si>
+  <si>
+    <t>Mozilla</t>
+  </si>
+  <si>
+    <t>LogIn_03</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>anshika@gmail.com</t>
+  </si>
+  <si>
+    <t>Iamking@000</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Page Name</t>
+  </si>
+  <si>
+    <t>Login_Page</t>
+  </si>
+  <si>
+    <t>Home_Page</t>
+  </si>
+  <si>
+    <t>Login_Page Objects</t>
+  </si>
+  <si>
+    <t>Home_Page Objects</t>
+  </si>
+  <si>
+    <t>btn_MyAccount</t>
+  </si>
+  <si>
+    <t>Action Keywords</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Enter any data</t>
+  </si>
+  <si>
+    <t>Click on buttons</t>
+  </si>
+  <si>
+    <t>Actions:</t>
+  </si>
+  <si>
+    <t>Asserts URL if it contains a specific string</t>
+  </si>
+  <si>
+    <t>assertURLContains</t>
+  </si>
+  <si>
+    <t>Assert Text Type</t>
+  </si>
+  <si>
+    <t>Contains</t>
+  </si>
+  <si>
+    <t>Equals</t>
+  </si>
+  <si>
+    <t>Startswith</t>
+  </si>
+  <si>
+    <t>Endswith</t>
+  </si>
+  <si>
+    <t>Assert Element Type</t>
+  </si>
+  <si>
+    <t>Assertions (text):</t>
+  </si>
+  <si>
+    <t>Assertions (Elements):</t>
+  </si>
+  <si>
+    <t>assertURLEQuals</t>
+  </si>
+  <si>
+    <t>asserts for expected and actual URL string</t>
+  </si>
+  <si>
+    <t>urlAssertCon</t>
+  </si>
+  <si>
+    <t>urlAssertEqu</t>
+  </si>
+  <si>
+    <t>Displayed</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Selected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +344,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +363,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,10 +449,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -321,8 +464,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -635,22 +783,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15D7A4B-A742-44BC-967B-448A7431389E}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="46.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -661,13 +812,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -678,11 +838,18 @@
         <v>18</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -693,11 +860,16 @@
         <v>19</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -707,14 +879,23 @@
       <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -724,14 +905,23 @@
       <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -741,14 +931,21 @@
       <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -759,11 +956,16 @@
         <v>24</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -774,13 +976,20 @@
         <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="4"/>
+      <c r="H8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -791,11 +1000,16 @@
         <v>24</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -806,13 +1020,18 @@
         <v>26</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
@@ -821,13 +1040,20 @@
         <v>18</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -836,13 +1062,18 @@
         <v>19</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -850,16 +1081,25 @@
       <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="D13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -867,16 +1107,25 @@
       <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -884,16 +1133,23 @@
       <c r="C15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
@@ -902,13 +1158,18 @@
         <v>24</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="6"/>
+      <c r="H16" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -917,15 +1178,22 @@
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" s="4"/>
+      <c r="H17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
@@ -934,13 +1202,18 @@
         <v>24</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
@@ -949,63 +1222,311 @@
         <v>26</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D28" xr:uid="{2FE79D81-8BB2-4290-93C7-D263E04CD2A3}">
+      <formula1>Page_name</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F28" xr:uid="{B242D20A-94AA-428B-89BE-D0BAA386714D}">
+      <formula1>Action_Keywords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E28" xr:uid="{5C953BEB-B207-4FA8-826C-90810C16B549}">
+      <formula1>INDIRECT(D2)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{60C8FF60-4AE3-4CC2-A01C-C50A2DBB8E77}"/>
+    <hyperlink ref="G13" r:id="rId2" xr:uid="{0C576929-D217-4A39-9FA5-3B0E9861AC8D}"/>
+    <hyperlink ref="G22" r:id="rId3" xr:uid="{6DE43C1D-12BC-4410-ADD4-0F9B123BCBF6}"/>
+    <hyperlink ref="G23" r:id="rId4" xr:uid="{D7433B66-72D8-4805-A33B-92442C0D349A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2B10FA-80A6-48E3-92E2-8BBA8BA0016C}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="46.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
+      <c r="D3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1015,6 +1536,313 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C605C9-9266-4AD3-89B7-BF5EE6DB9E58}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75369D15-EC67-43EA-98A5-A7131518D7B8}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A10" xr:uid="{C7929CFB-004A-4259-9F7F-B8928E892768}">
+      <formula1>Action_Keywords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C10" xr:uid="{8D22B27F-B950-4707-8DBE-2ED2CB8F43F3}">
+      <formula1>INDIRECT(B3)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48220B37-1FBB-4A15-A1B5-5A91E86F14AE}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1070,7 +1898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638BEB8B-0C06-4187-B1B0-0DABDCBA5665}">
   <dimension ref="A1:D10"/>
   <sheetViews>

</xml_diff>